<commit_message>
change notes file to csv
</commit_message>
<xml_diff>
--- a/data/esg_metadata_notes.xlsx
+++ b/data/esg_metadata_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/acastanedaa_worldbank_org/Documents/WorldBank/DECDG/ESG/ESG_availability/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{B1578202-5D52-4CC3-B6FD-082E4B133B5B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{BEEF6ED1-C846-4F0B-B564-B139DF036AAF}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{B1578202-5D52-4CC3-B6FD-082E4B133B5B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{95EDC21A-1A49-46D2-8F5A-CB395692C97F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D19A9FAE-F0B3-4A28-B5FE-529B16A7192A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="419">
   <si>
     <t>cetsid</t>
   </si>
@@ -1548,6 +1548,18 @@
   </si>
   <si>
     <t xml:space="preserve">Overall budget surplus/deficit (excluding current grants) is current and capital revenue excluding current grants, less total expenditure and lending minus repayments. Data are shown for central government only, and are in current local currency.  </t>
+  </si>
+  <si>
+    <t>other_notes</t>
+  </si>
+  <si>
+    <t>Data are projections for 2040-2059</t>
+  </si>
+  <si>
+    <t>Data are projections for 2040-2059.</t>
+  </si>
+  <si>
+    <t>Data retrieved via API in March 2019. For detailed information on the observation level (e.g. National Estimation, UIS Estimation, or Category not applicable), please visit UIS.Stat (http://data.uis.unesco.org/).</t>
   </si>
 </sst>
 </file>
@@ -1901,15 +1913,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38DD77A9-6EEC-4FEB-BFCB-834F98C04471}">
-  <dimension ref="A1:H139"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1934,8 +1946,11 @@
       <c r="H1" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1952,7 +1967,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1969,7 +1984,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1986,7 +2001,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2003,7 +2018,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2020,7 +2035,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2037,7 +2052,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2045,7 +2060,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2059,7 +2074,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2073,7 +2088,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2093,7 +2108,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2107,7 +2122,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2127,7 +2142,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2147,7 +2162,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2167,7 +2182,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2178,7 +2193,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2189,7 +2204,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2200,7 +2215,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2220,12 +2235,12 @@
         <v>369</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2242,7 +2257,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2259,7 +2274,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2273,47 +2288,56 @@
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -2482,7 +2506,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -2499,7 +2523,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -2507,7 +2531,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -2524,7 +2548,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -2541,7 +2565,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -2554,8 +2578,11 @@
       <c r="D53" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -2572,7 +2599,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -2589,7 +2616,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -2602,8 +2629,11 @@
       <c r="D56" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -2616,8 +2646,11 @@
       <c r="D57" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -2630,8 +2663,11 @@
       <c r="D58" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -2644,8 +2680,11 @@
       <c r="D59" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -2658,8 +2697,11 @@
       <c r="D60" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -2676,7 +2718,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -2693,7 +2735,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -2707,7 +2749,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -3145,7 +3187,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>94</v>
       </c>
@@ -3153,7 +3195,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -3170,7 +3212,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>96</v>
       </c>
@@ -3181,7 +3223,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>97</v>
       </c>
@@ -3189,7 +3231,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>98</v>
       </c>
@@ -3200,7 +3242,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>99</v>
       </c>
@@ -3214,7 +3256,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>100</v>
       </c>
@@ -3222,7 +3264,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>101</v>
       </c>
@@ -3230,7 +3272,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>102</v>
       </c>
@@ -3238,7 +3280,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>103</v>
       </c>
@@ -3246,7 +3288,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>104</v>
       </c>
@@ -3259,18 +3301,21 @@
       <c r="D107" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>107</v>
       </c>
@@ -3281,7 +3326,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>108</v>
       </c>
@@ -3289,12 +3334,12 @@
         <v>408</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>110</v>
       </c>
@@ -3311,7 +3356,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>111</v>
       </c>
@@ -3327,8 +3372,11 @@
       <c r="G114" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I114" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>112</v>
       </c>
@@ -3342,7 +3390,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>113</v>
       </c>
@@ -3365,7 +3413,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>114</v>
       </c>
@@ -3376,7 +3424,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>115</v>
       </c>
@@ -3387,7 +3435,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>116</v>
       </c>
@@ -3397,8 +3445,11 @@
       <c r="C119" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I119" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>117</v>
       </c>
@@ -3415,7 +3466,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>118</v>
       </c>
@@ -3426,7 +3477,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>119</v>
       </c>
@@ -3446,7 +3497,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>120</v>
       </c>
@@ -3463,7 +3514,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>121</v>
       </c>
@@ -3480,7 +3531,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>122</v>
       </c>
@@ -3488,7 +3539,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -3505,12 +3556,12 @@
         <v>395</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>125</v>
       </c>
@@ -3521,7 +3572,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>126</v>
       </c>
@@ -3532,7 +3583,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>127</v>
       </c>
@@ -3552,7 +3603,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>128</v>
       </c>
@@ -3569,7 +3620,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>129</v>
       </c>
@@ -3579,8 +3630,11 @@
       <c r="C132" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>130</v>
       </c>
@@ -3594,7 +3648,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>131</v>
       </c>
@@ -3611,7 +3665,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>132</v>
       </c>
@@ -3621,8 +3675,11 @@
       <c r="D135" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I135" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>133</v>
       </c>
@@ -3632,8 +3689,11 @@
       <c r="D136" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I136" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>134</v>
       </c>
@@ -3650,12 +3710,12 @@
         <v>398</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>136</v>
       </c>
@@ -3666,21 +3726,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007787EA3DE823DC489E44BF4CD2C2AF9F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a73e9e290f0f235d52559cf13ce0f416">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="543abfbf-1b39-4535-8b1b-c72a4cdaa484" xmlns:ns4="2834bc84-a818-4cb9-8b4d-5179cfe104eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="14c961546e2089148b65b867a2b76298" ns3:_="" ns4:_="">
     <xsd:import namespace="543abfbf-1b39-4535-8b1b-c72a4cdaa484"/>
@@ -3903,32 +3948,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9B912E8-5FC9-43AE-B295-362E6F9B19D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="543abfbf-1b39-4535-8b1b-c72a4cdaa484"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2834bc84-a818-4cb9-8b4d-5179cfe104eb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC92196A-B058-488F-AD01-E0BF41C1A61C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D0D69B5-4932-4C62-B395-3B5820C83728}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3945,4 +3980,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC92196A-B058-488F-AD01-E0BF41C1A61C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9B912E8-5FC9-43AE-B295-362E6F9B19D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="543abfbf-1b39-4535-8b1b-c72a4cdaa484"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2834bc84-a818-4cb9-8b4d-5179cfe104eb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>